<commit_message>
feat: update Scene table
</commit_message>
<xml_diff>
--- a/dragon-verse/Excels/Scene_场景表.xlsx
+++ b/dragon-verse/Excels/Scene_场景表.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>int</t>
   </si>
@@ -33,6 +33,9 @@
     <t>name</t>
   </si>
   <si>
+    <t>foreshow</t>
+  </si>
+  <si>
     <t>bornAreaId</t>
   </si>
   <si>
@@ -46,6 +49,9 @@
   </si>
   <si>
     <t>场景名称（多语言表key）</t>
+  </si>
+  <si>
+    <t>传送预告内容</t>
   </si>
   <si>
     <t xml:space="preserve">出生点区域 ID</t>
@@ -118,7 +124,7 @@
     <numFmt numFmtId="162" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="163" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="22">
     <font>
       <sz val="10.000000"/>
       <color theme="1"/>
@@ -255,11 +261,6 @@
     </font>
     <font>
       <sz val="10.000000"/>
-      <name val="微软雅黑"/>
-    </font>
-    <font>
-      <sz val="10.000000"/>
-      <color indexed="64"/>
       <name val="微软雅黑"/>
     </font>
   </fonts>
@@ -701,7 +702,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyProtection="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1" applyProtection="1">
@@ -716,16 +717,28 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf fontId="21" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="21" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf fontId="22" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf fontId="21" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf fontId="21" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -827,13 +840,13 @@
         <color theme="1"/>
       </font>
       <border>
-        <left/>
-        <right/>
+        <left style="none"/>
+        <right style="none"/>
         <top style="double">
           <color theme="4"/>
         </top>
-        <bottom/>
-        <diagonal/>
+        <bottom style="none"/>
+        <diagonal style="none"/>
       </border>
     </dxf>
     <dxf>
@@ -853,7 +866,7 @@
         <bottom style="thin">
           <color theme="4"/>
         </bottom>
-        <diagonal/>
+        <diagonal style="none"/>
         <horizontal style="thin">
           <color theme="4" tint="0.39997558519241899"/>
         </horizontal>
@@ -880,13 +893,13 @@
         <color theme="1"/>
       </font>
       <border>
-        <left/>
-        <right/>
-        <top/>
+        <left style="none"/>
+        <right style="none"/>
+        <top style="none"/>
         <bottom style="thin">
           <color theme="4" tint="0.39997558519241899"/>
         </bottom>
-        <diagonal/>
+        <diagonal style="none"/>
       </border>
     </dxf>
     <dxf>
@@ -895,15 +908,15 @@
         <color theme="1"/>
       </font>
       <border>
-        <left/>
-        <right/>
+        <left style="none"/>
+        <right style="none"/>
         <top style="thin">
           <color theme="4"/>
         </top>
         <bottom style="thin">
           <color theme="4"/>
         </bottom>
-        <diagonal/>
+        <diagonal style="none"/>
       </border>
     </dxf>
     <dxf>
@@ -918,13 +931,13 @@
         </patternFill>
       </fill>
       <border>
-        <left/>
-        <right/>
-        <top/>
+        <left style="none"/>
+        <right style="none"/>
+        <top style="none"/>
         <bottom style="thin">
           <color theme="4" tint="0.39997558519241899"/>
         </bottom>
-        <diagonal/>
+        <diagonal style="none"/>
       </border>
     </dxf>
     <dxf>
@@ -938,13 +951,13 @@
         </patternFill>
       </fill>
       <border>
-        <left/>
-        <right/>
-        <top/>
+        <left style="none"/>
+        <right style="none"/>
+        <top style="none"/>
         <bottom style="thin">
           <color theme="4" tint="0.39997558519241899"/>
         </bottom>
-        <diagonal/>
+        <diagonal style="none"/>
       </border>
     </dxf>
     <dxf>
@@ -955,13 +968,13 @@
         </patternFill>
       </fill>
       <border>
-        <left/>
-        <right/>
-        <top/>
+        <left style="none"/>
+        <right style="none"/>
+        <top style="none"/>
         <bottom style="thin">
           <color theme="4" tint="0.39997558519241899"/>
         </bottom>
-        <diagonal/>
+        <diagonal style="none"/>
       </border>
     </dxf>
     <dxf>
@@ -987,15 +1000,15 @@
         </patternFill>
       </fill>
       <border>
-        <left/>
-        <right/>
+        <left style="none"/>
+        <right style="none"/>
         <top style="thin">
           <color theme="4" tint="0.39997558519241899"/>
         </top>
         <bottom style="thin">
           <color theme="4" tint="0.39997558519241899"/>
         </bottom>
-        <diagonal/>
+        <diagonal style="none"/>
       </border>
     </dxf>
   </dxfs>
@@ -1534,15 +1547,15 @@
   <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15"/>
   <cols>
     <col customWidth="1" min="1" max="1" style="1" width="30.75390625"/>
-    <col customWidth="1" min="2" max="2" style="1" width="51.858333333333299"/>
-    <col customWidth="1" min="3" max="3" style="2" width="25.066666666666698"/>
-    <col customWidth="1" min="4" max="4" style="1" width="17.141666666666701"/>
-    <col customWidth="1" min="5" max="5" style="1" width="18.375"/>
-    <col customWidth="1" min="6" max="6" style="1" width="16.658333333333299"/>
-    <col customWidth="1" min="11" max="11" style="1" width="13.1916666666667"/>
-    <col customWidth="1" min="12" max="12" style="1" width="14.1833333333333"/>
-    <col customWidth="1" min="14" max="14" style="1" width="34.308333333333302"/>
-    <col customWidth="1" min="15" max="15" style="1" width="24.091666666666701"/>
+    <col customWidth="1" min="2" max="3" style="1" width="51.858333333333299"/>
+    <col customWidth="1" min="4" max="4" style="2" width="25.066666666666698"/>
+    <col customWidth="1" min="5" max="5" style="1" width="17.141666666666701"/>
+    <col customWidth="1" min="6" max="6" style="1" width="18.375"/>
+    <col customWidth="1" min="7" max="7" style="1" width="16.658333333333299"/>
+    <col customWidth="1" min="12" max="12" style="1" width="13.1916666666667"/>
+    <col customWidth="1" min="13" max="13" style="1" width="14.1833333333333"/>
+    <col customWidth="1" min="15" max="15" style="1" width="34.308333333333302"/>
+    <col customWidth="1" min="16" max="16" style="1" width="24.091666666666701"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="1">
@@ -1553,15 +1566,18 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1575,59 +1591,68 @@
       <c r="C2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="S2" s="4"/>
+      <c r="G2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="T2" s="4"/>
     </row>
     <row r="3" s="3" customFormat="1" ht="23.25" customHeight="1">
       <c r="B3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="C3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="E3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="4"/>
+      <c r="F3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="P3" s="4"/>
     </row>
     <row r="4" s="2" customFormat="1">
-      <c r="B4" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="B4" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="9"/>
     </row>
     <row r="5" s="2" customFormat="1">
       <c r="A5" s="2">
         <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="8">
+        <v>18</v>
+      </c>
+      <c r="C5" s="10"/>
+      <c r="E5" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="6" s="2" customFormat="1">
-      <c r="A6" s="8">
+      <c r="A6" s="11">
         <v>2</v>
       </c>
-      <c r="B6" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="8">
+      <c r="B6" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="13"/>
+      <c r="E6" s="11">
         <v>2</v>
       </c>
     </row>
@@ -1635,21 +1660,23 @@
       <c r="A7" s="2">
         <v>3</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="8">
+      <c r="B7" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="13"/>
+      <c r="E7" s="11">
         <v>3</v>
       </c>
     </row>
     <row r="8" s="2" customFormat="1">
-      <c r="A8" s="8">
+      <c r="A8" s="11">
         <v>4</v>
       </c>
-      <c r="B8" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="8">
+      <c r="B8" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="13"/>
+      <c r="E8" s="11">
         <v>4</v>
       </c>
     </row>
@@ -1657,21 +1684,23 @@
       <c r="A9" s="2">
         <v>5</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="8">
+      <c r="B9" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="13"/>
+      <c r="E9" s="11">
         <v>5</v>
       </c>
     </row>
     <row r="10" s="2" customFormat="1">
-      <c r="A10" s="8">
+      <c r="A10" s="11">
         <v>6</v>
       </c>
-      <c r="B10" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="8">
+      <c r="B10" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="13"/>
+      <c r="E10" s="11">
         <v>6</v>
       </c>
     </row>
@@ -1679,10 +1708,11 @@
       <c r="A11" s="2">
         <v>7</v>
       </c>
-      <c r="B11" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="8">
+      <c r="B11" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="13"/>
+      <c r="E11" s="11">
         <v>7</v>
       </c>
     </row>
@@ -1691,88 +1721,89 @@
         <v>8</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="8"/>
+        <v>25</v>
+      </c>
+      <c r="C12" s="10"/>
+      <c r="E12" s="11"/>
     </row>
     <row r="13" s="2" customFormat="1"/>
     <row r="14" s="2" customFormat="1">
-      <c r="C14" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
+      <c r="D14" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
     </row>
     <row r="15" s="2" customFormat="1">
-      <c r="C15" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
+      <c r="D15" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
     </row>
     <row r="16" s="2" customFormat="1">
-      <c r="C16" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
+      <c r="D16" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
     </row>
     <row r="17" s="2" customFormat="1">
-      <c r="C17" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
+      <c r="D17" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
     </row>
     <row r="18" s="2" customFormat="1">
-      <c r="C18" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
+      <c r="D18" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
     </row>
     <row r="19" s="2" customFormat="1">
-      <c r="C19" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
+      <c r="D19" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
     </row>
     <row r="20" s="2" customFormat="1">
-      <c r="C20" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
+      <c r="D20" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
     </row>
     <row r="21" s="2" customFormat="1">
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
     </row>
     <row r="22" s="2" customFormat="1"/>
     <row r="23" s="2" customFormat="1"/>
@@ -1780,10 +1811,10 @@
     <row r="25" s="2" customFormat="1"/>
     <row r="26" s="2" customFormat="1"/>
     <row r="27" s="2" customFormat="1">
-      <c r="C27" s="8"/>
+      <c r="D27" s="11"/>
     </row>
     <row r="28" s="2" customFormat="1">
-      <c r="C28" s="8"/>
+      <c r="D28" s="11"/>
     </row>
     <row r="29" s="2" customFormat="1"/>
     <row r="30" s="2" customFormat="1"/>

</xml_diff>

<commit_message>
feat：update scene excel change
</commit_message>
<xml_diff>
--- a/dragon-verse/Excels/Scene_场景表.xlsx
+++ b/dragon-verse/Excels/Scene_场景表.xlsx
@@ -125,9 +125,6 @@
     <t xml:space="preserve">Main_Scene_Name11</t>
   </si>
   <si>
-    <t xml:space="preserve">Main_Scene_Name12</t>
-  </si>
-  <si>
     <t xml:space="preserve">Main_Scene_Name13</t>
   </si>
   <si>
@@ -147,6 +144,9 @@
   </si>
   <si>
     <t xml:space="preserve">Main_Scene_Name19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Main_Scene_Name20</t>
   </si>
   <si>
     <t xml:space="preserve">MaxLanItemCount</t>
@@ -495,7 +495,7 @@
   <dimension ref="A1:U500"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
+      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75390625" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
feat：update character and tip change
</commit_message>
<xml_diff>
--- a/dragon-verse/Excels/Scene_场景表.xlsx
+++ b/dragon-verse/Excels/Scene_场景表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="42">
   <si>
     <t xml:space="preserve">int</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t xml:space="preserve">Language</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tiptext007</t>
   </si>
   <si>
     <t xml:space="preserve">Main_Scene_Name</t>
@@ -495,7 +498,7 @@
   <dimension ref="A1:U500"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75390625" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -632,17 +635,23 @@
       <c r="B4" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="D4" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="5" s="2" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="n">
         <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C5" s="2" t="str">
         <f aca="true" t="array" ref="C5:C5">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B5,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="2" t="n">
@@ -660,13 +669,15 @@
         <v>2</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C6" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B6,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D6" s="7"/>
+      <c r="D6" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="E6" s="7" t="n">
         <v>22</v>
       </c>
@@ -685,13 +696,15 @@
         <v>3</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C7" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B7,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D7" s="7"/>
+      <c r="D7" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="E7" s="7" t="n">
         <v>23</v>
       </c>
@@ -710,13 +723,15 @@
         <v>4</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C8" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B8,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D8" s="7"/>
+      <c r="D8" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="E8" s="7" t="n">
         <v>24</v>
       </c>
@@ -724,7 +739,7 @@
         <v>4</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H8" s="2" t="n">
         <v>7</v>
@@ -735,13 +750,15 @@
         <v>5</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C9" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B9,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D9" s="7"/>
+      <c r="D9" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="E9" s="7" t="n">
         <v>25</v>
       </c>
@@ -760,13 +777,15 @@
         <v>6</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C10" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B10,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D10" s="7"/>
+      <c r="D10" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="E10" s="7" t="n">
         <v>26</v>
       </c>
@@ -785,13 +804,15 @@
         <v>7</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C11" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B11,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D11" s="7"/>
+      <c r="D11" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="E11" s="7" t="n">
         <v>27</v>
       </c>
@@ -814,6 +835,9 @@
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B12,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
+      <c r="D12" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="E12" s="2" t="n">
         <v>28</v>
       </c>
@@ -823,11 +847,14 @@
         <v>9</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C13" s="2" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B13,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="E13" s="2" t="n">
         <v>42</v>
@@ -847,11 +874,14 @@
         <v>10</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C14" s="2" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B14,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="E14" s="2" t="n">
         <v>43</v>
@@ -871,11 +901,14 @@
         <v>11</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C15" s="2" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B15,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="E15" s="2" t="n">
         <v>44</v>
@@ -895,11 +928,14 @@
         <v>12</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C16" s="2" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B16,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="E16" s="2" t="n">
         <v>45</v>
@@ -919,11 +955,14 @@
         <v>13</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C17" s="2" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B17,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="E17" s="2" t="n">
         <v>46</v>
@@ -943,11 +982,14 @@
         <v>14</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C18" s="2" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B18,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="E18" s="2" t="n">
         <v>47</v>
@@ -967,11 +1009,14 @@
         <v>15</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C19" s="2" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B19,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="E19" s="2" t="n">
         <v>48</v>
@@ -991,11 +1036,14 @@
         <v>16</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C20" s="2" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B20,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="E20" s="2" t="n">
         <v>49</v>
@@ -1015,11 +1063,14 @@
         <v>17</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C21" s="2" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B21,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="E21" s="2" t="n">
         <v>50</v>
@@ -1039,11 +1090,14 @@
         <v>18</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C22" s="2" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B22,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="E22" s="2" t="n">
         <v>51</v>
@@ -1063,11 +1117,14 @@
         <v>19</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C23" s="2" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B23,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="E23" s="2" t="n">
         <v>52</v>
@@ -1087,11 +1144,14 @@
         <v>20</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C24" s="2" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B24,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="E24" s="2" t="n">
         <v>53</v>
@@ -1111,11 +1171,14 @@
         <v>21</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C25" s="2" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B25,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="E25" s="2" t="n">
         <v>54</v>
@@ -4269,7 +4332,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B1" s="1" t="n">
         <v>500</v>

</xml_diff>